<commit_message>
Override VS Overload     *******   this VS super 作用域
</commit_message>
<xml_diff>
--- a/dayLog/检查清单.xlsx
+++ b/dayLog/检查清单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workPlace\java20190119\dayLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F67E46-B610-4B28-BF33-BD8575CE7272}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4187E8BF-2249-458D-8821-8B6B1540674C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1935" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27405" yWindow="2655" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>Java 教程</t>
   </si>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -805,6 +805,12 @@
       <c r="C12">
         <v>10</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F12" s="4">
         <v>43518</v>
       </c>
@@ -816,6 +822,12 @@
       <c r="C13">
         <v>11</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F13" s="4">
         <v>43518</v>
       </c>
@@ -827,6 +839,12 @@
       <c r="C14">
         <v>12</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F14" s="4">
         <v>43518</v>
       </c>
@@ -838,6 +856,12 @@
       <c r="C15">
         <v>13</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F15" s="4">
         <v>43518</v>
       </c>
@@ -849,6 +873,12 @@
       <c r="C16">
         <v>14</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F16" s="4">
         <v>43518</v>
       </c>
@@ -860,6 +890,12 @@
       <c r="C17">
         <v>15</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F17" s="4">
         <v>43518</v>
       </c>
@@ -871,6 +907,15 @@
       <c r="C18">
         <v>16</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="4">
+        <v>43519</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
@@ -879,6 +924,15 @@
       <c r="C19">
         <v>17</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="4">
+        <v>43519</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
@@ -887,6 +941,15 @@
       <c r="C20">
         <v>18</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="4">
+        <v>43521</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
@@ -895,6 +958,9 @@
       <c r="C21">
         <v>19</v>
       </c>
+      <c r="F21" s="4">
+        <v>43521</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
@@ -903,6 +969,9 @@
       <c r="C22">
         <v>20</v>
       </c>
+      <c r="F22" s="4">
+        <v>43521</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
@@ -911,6 +980,9 @@
       <c r="C23">
         <v>21</v>
       </c>
+      <c r="F23" s="4">
+        <v>43521</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
@@ -919,6 +991,9 @@
       <c r="C24">
         <v>22</v>
       </c>
+      <c r="F24" s="4">
+        <v>43521</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
@@ -931,6 +1006,9 @@
       </c>
       <c r="C28">
         <v>23</v>
+      </c>
+      <c r="F28" s="4">
+        <v>43522</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>